<commit_message>
melhorias no codigo, chance de acerto do move e controle do clima
</commit_message>
<xml_diff>
--- a/Entities/Data/ItemCard.xlsx
+++ b/Entities/Data/ItemCard.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16125" windowHeight="10530"/>
+    <workbookView windowWidth="21195" windowHeight="11115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="135">
   <si>
     <t>ID</t>
   </si>
@@ -50,13 +50,13 @@
     <t>Name PT</t>
   </si>
   <si>
-    <t>Guard Esp.</t>
+    <t>Guard Spec.</t>
   </si>
   <si>
     <t>Battle</t>
   </si>
   <si>
-    <t>W.IMUNE.B.TWODICE</t>
+    <t>W.IMMUNE.B.TWODICE</t>
   </si>
   <si>
     <t>Uncommon</t>
@@ -146,6 +146,9 @@
     <t>Recuperação Completa</t>
   </si>
   <si>
+    <t>Dire Hit</t>
+  </si>
+  <si>
     <t>W.DICESIDE.8</t>
   </si>
   <si>
@@ -155,10 +158,13 @@
     <t>Golpe Difícil</t>
   </si>
   <si>
+    <t>Air Balloon</t>
+  </si>
+  <si>
     <t>Attach</t>
   </si>
   <si>
-    <t>IMMUNE.GROUND;B.POWERMOVE.GROUND.0</t>
+    <t>A.IMMUNE.GROUND</t>
   </si>
   <si>
     <t>The power of ground-type moves' from your opponent's Pokémon is 0, and the Pokémon attached to this card cannot be affected by its effects.</t>
@@ -167,7 +173,10 @@
     <t>Balão de Ar</t>
   </si>
   <si>
-    <t>IMMUNE.TRAPCARD</t>
+    <t>Heavy-Duty Boots</t>
+  </si>
+  <si>
+    <t>A.IMMUNE.TRAPCARD</t>
   </si>
   <si>
     <t>The Pokémon attached to this card is not affected by Trap Cards on the field.</t>
@@ -176,7 +185,10 @@
     <t>Botas Grossas</t>
   </si>
   <si>
-    <t>ADDEFFECT.W.TWODICES.ONCE</t>
+    <t>Assault Vest</t>
+  </si>
+  <si>
+    <t>A.ADDEFFECT.W.TWODICES.ONCE</t>
   </si>
   <si>
     <t>Once per battle, the attached Pokémon's move gains: Advantage (if you roll 5 or more on the effect die)</t>
@@ -188,7 +200,7 @@
     <t>Exp. Share</t>
   </si>
   <si>
-    <t>EXPSHARE</t>
+    <t>A.EXPSHARE</t>
   </si>
   <si>
     <t>Once per battle, if a Pokémon levels up, you may instead place the level on this attached Pokémon, provided that the defeated Pokémon has a level equal to or higher than this Pokémon.</t>
@@ -197,10 +209,21 @@
     <t>Compartilhar Exp.</t>
   </si>
   <si>
-    <t>BERRY.EFFECTIVE;ADDROLL.2</t>
+    <t>Enigma Berry</t>
+  </si>
+  <si>
+    <t>B.EFFECTIVE;W.ADDROLL.2</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Berry:</t>
     </r>
     <r>
@@ -221,10 +244,18 @@
     <t>Lum Berry</t>
   </si>
   <si>
-    <t>BERRY.STATUS;HEAL.STATUS</t>
+    <t>B.STATUS;W.HEAL.STATUS</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Berry:</t>
     </r>
     <r>
@@ -245,10 +276,18 @@
     <t>Oran Berry</t>
   </si>
   <si>
-    <t>BERRY.ROLL;ADDPOWER.1</t>
+    <t>B.ROLL;W.ADDPOWER.1</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Berry: </t>
     </r>
     <r>
@@ -269,10 +308,18 @@
     <t>Sitrus Berry</t>
   </si>
   <si>
-    <t>BERRY.ROLL;ADDPOWER.3</t>
+    <t>B.ROLL;W.ADDPOWER.3</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Berry: </t>
     </r>
     <r>
@@ -290,7 +337,10 @@
     <t>Fruta Sitrus</t>
   </si>
   <si>
-    <t>ADDEFFECT.W.DICESIDE.8.ONCE</t>
+    <t>Razor Claw</t>
+  </si>
+  <si>
+    <t>A.ADDEFFECT.W.DICESIDE.8.ONCE</t>
   </si>
   <si>
     <t>Once per battle, a move of the Pokémon attached to this card has d8. It can reduce the evolution cost of specific Pokémon.</t>
@@ -302,7 +352,7 @@
     <t>Choice Scarf</t>
   </si>
   <si>
-    <t>BLOCKMOVE;ADDEFFECT.TWODICES</t>
+    <t>A.BLOCKMOVE;A.ADDEFFECT.TWODICES</t>
   </si>
   <si>
     <t>The Pokémon attached to this card can only use a single move during the battle. That move has an advantage.</t>
@@ -311,7 +361,10 @@
     <t>Lenço Escolha</t>
   </si>
   <si>
-    <t>COND.POISON;ADDEFFECT.LIFE.5</t>
+    <t>Black Sludge</t>
+  </si>
+  <si>
+    <t>A.TYPE.POISON;A.ADDEFFECT.LIFE.5</t>
   </si>
   <si>
     <t>If the Pokémon attached to this card is Poison type, its moves have Life if you roll a 5 on the effect die.</t>
@@ -323,7 +376,7 @@
     <t>Amulet Coin</t>
   </si>
   <si>
-    <t>REWARD;DRAW.1;DISCARD.1</t>
+    <t>A.REWARD;W.DRAW.1;W.DISCARD.1</t>
   </si>
   <si>
     <t>When you draw an Item card with the battle reward, you can buy 1 additional one and discard the card from your hand.</t>
@@ -332,7 +385,10 @@
     <t>Moeda Amuleto</t>
   </si>
   <si>
-    <t>BLOCKMOVE;ADDEFFECT.PRECISION</t>
+    <t>Choice Specs</t>
+  </si>
+  <si>
+    <t>A.BLOCKMOVE;W.ADDEFFECT.PRECISION</t>
   </si>
   <si>
     <t>The Pokémon attached to this card can only use a single move during the battle. That move has precision.</t>
@@ -344,7 +400,7 @@
     <t>Toxic Orb</t>
   </si>
   <si>
-    <t>ADDEFFECT.POISON.5.ONCE</t>
+    <t>A.ADDEFFECT.POISON.5.ONCE</t>
   </si>
   <si>
     <t>Once per battle, the move of the attached Pokémon gains: Poison if 5 or more is rolled on the effect die.</t>
@@ -356,7 +412,7 @@
     <t>Flame Orb</t>
   </si>
   <si>
-    <t>ADDEFFECT.BURN.5.ONCE</t>
+    <t>A.ADDEFFECT.BURN.5.ONCE</t>
   </si>
   <si>
     <t>Once per battle, the move of the attached Pokémon gains: Burn if 5 or more is rolled on the effect die.</t>
@@ -377,7 +433,7 @@
     <t>Heat Rock</t>
   </si>
   <si>
-    <t>SUNNYDAY</t>
+    <t>A.SUNNYDAY</t>
   </si>
   <si>
     <t>When the Pokémon attached to this card enters play, activate the weather effect: Sunny Day</t>
@@ -389,7 +445,7 @@
     <t>King Rock</t>
   </si>
   <si>
-    <t>ADDEFFECT.B.TWODICES.6.ONCE</t>
+    <t>A.ADDEFFECT.B.TWODICES.6.ONCE</t>
   </si>
   <si>
     <t>Once per battle, a move of the Pokémon attached to this card has the opponent at a disadvantage if 6. It can reduce the evolution cost of specific Pokémon.</t>
@@ -398,7 +454,10 @@
     <t>Pedra do Rei</t>
   </si>
   <si>
-    <t>SNOW</t>
+    <t>Icy Rock</t>
+  </si>
+  <si>
+    <t>A.SNOW</t>
   </si>
   <si>
     <t>When the Pokémon attached to this card enters play, activate the weather effect: Snow</t>
@@ -407,7 +466,10 @@
     <t>Pedra Gelada</t>
   </si>
   <si>
-    <t>SANDSTORM</t>
+    <t>Smooth Rock</t>
+  </si>
+  <si>
+    <t>A.SAND</t>
   </si>
   <si>
     <t>When the Pokémon attached to this card enters play, activate the weather effect: Sandstorm</t>
@@ -416,7 +478,10 @@
     <t>Pedra Lisa</t>
   </si>
   <si>
-    <t>RAIN</t>
+    <t>Damp Rock</t>
+  </si>
+  <si>
+    <t>A.RAIN</t>
   </si>
   <si>
     <t>When the Pokémon attached to this card enters play, activate the weather effect: Rain</t>
@@ -425,7 +490,10 @@
     <t>Pedra Úmida</t>
   </si>
   <si>
-    <t>REROLL.EFFECTDICE.ONCE</t>
+    <t>Blunder Policy</t>
+  </si>
+  <si>
+    <t>A.REROLL.REDDICE.ONCE</t>
   </si>
   <si>
     <t>Once per battle, the Pokémon attached to this card rolls an effect die and fails, roll again.</t>
@@ -434,10 +502,10 @@
     <t>Seguro Contra Erro</t>
   </si>
   <si>
-    <t>VITAMIN</t>
-  </si>
-  <si>
-    <t>ADDROLL.1</t>
+    <t>Vitamin</t>
+  </si>
+  <si>
+    <t>A.ADDROLL.1</t>
   </si>
   <si>
     <t>Increase by 1 all attack rolls that the attached Pokémon makes.</t>
@@ -1160,7 +1228,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:G32" totalsRowShown="0">
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G32" etc:filterBottomFollowUsedRange="0"/>
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G32" etc:filterBottomFollowUsedRange="0">
+    <filterColumn colId="2">
+      <customFilters>
+        <customFilter operator="equal" val="Attach"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="7">
     <tableColumn id="1" name="ID" dataDxfId="0"/>
     <tableColumn id="2" name="Name" dataDxfId="1"/>
@@ -1434,15 +1508,15 @@
   <sheetPr/>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="4.71428571428571" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="1"/>
+    <col min="2" max="2" width="18.1428571428571" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28571428571429" style="1" customWidth="1"/>
     <col min="4" max="4" width="44.5714285714286" style="2" customWidth="1"/>
     <col min="5" max="5" width="19.8571428571429" style="2" customWidth="1"/>
     <col min="6" max="6" width="50.5714285714286" style="1" customWidth="1"/>
@@ -1473,7 +1547,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" ht="45" spans="1:7">
+    <row r="2" ht="45" hidden="1" spans="1:7">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1496,7 +1570,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" hidden="1" spans="1:7">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1519,7 +1593,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" hidden="1" spans="1:7">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1542,7 +1616,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" hidden="1" spans="1:7">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1565,7 +1639,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" hidden="1" spans="1:7">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1588,7 +1662,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" ht="30" hidden="1" spans="1:7">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1611,7 +1685,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" ht="30" spans="1:7">
+    <row r="8" ht="30" hidden="1" spans="1:7">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1634,86 +1708,96 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" ht="30" spans="1:7">
+    <row r="9" ht="30" hidden="1" spans="1:7">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" ht="45" spans="1:7">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="C10" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" ht="30" spans="1:7">
       <c r="A11" s="1">
         <v>10</v>
       </c>
+      <c r="B11" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" ht="30" spans="1:7">
       <c r="A12" s="1">
         <v>11</v>
       </c>
+      <c r="B12" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="C12" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" ht="60" spans="1:7">
@@ -1721,42 +1805,45 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" ht="45" spans="1:7">
       <c r="A14" s="1">
         <v>13</v>
       </c>
+      <c r="B14" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="C14" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" ht="60" spans="1:7">
@@ -1764,22 +1851,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" ht="45" spans="1:7">
@@ -1787,22 +1874,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" ht="45" spans="1:7">
@@ -1810,42 +1897,45 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" ht="45" spans="1:7">
       <c r="A18" s="1">
         <v>17</v>
       </c>
+      <c r="B18" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="C18" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" ht="30" spans="1:7">
@@ -1853,42 +1943,45 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" ht="30" spans="1:7">
       <c r="A20" s="1">
         <v>19</v>
       </c>
+      <c r="B20" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="C20" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" ht="45" spans="1:7">
@@ -1896,42 +1989,45 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" ht="30" spans="1:7">
       <c r="A22" s="1">
         <v>21</v>
       </c>
+      <c r="B22" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="C22" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" ht="30" spans="1:7">
@@ -1939,22 +2035,22 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" ht="30" spans="1:7">
@@ -1962,22 +2058,22 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" ht="45" spans="1:7">
@@ -1985,22 +2081,22 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" ht="30" spans="1:7">
@@ -2008,22 +2104,22 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" ht="45" spans="1:7">
@@ -2031,102 +2127,114 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" ht="30" spans="1:7">
       <c r="A28" s="1">
         <v>27</v>
       </c>
+      <c r="B28" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="C28" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" ht="30" spans="1:7">
       <c r="A29" s="1">
         <v>28</v>
       </c>
+      <c r="B29" s="1" t="s">
+        <v>119</v>
+      </c>
       <c r="C29" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" ht="30" spans="1:7">
       <c r="A30" s="1">
         <v>29</v>
       </c>
+      <c r="B30" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="C30" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" ht="30" spans="1:7">
       <c r="A31" s="1">
         <v>30</v>
       </c>
+      <c r="B31" s="1" t="s">
+        <v>127</v>
+      </c>
       <c r="C31" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32" ht="30" spans="1:7">
@@ -2134,22 +2242,22 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>24</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>